<commit_message>
Code updated for gold rate test case
</commit_message>
<xml_diff>
--- a/Output/TestResult.xlsx
+++ b/Output/TestResult.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ibmadmin\PycharmProjects\MoneyControl\Output\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="80" windowWidth="20120" windowHeight="8000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Currency" sheetId="1" r:id="rId1"/>
+    <sheet name="Gold Price" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Currency Name</t>
   </si>
@@ -68,12 +74,24 @@
   </si>
   <si>
     <t>2.6397</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Change</t>
+  </si>
+  <si>
+    <t>%Change</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -120,6 +138,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -168,7 +189,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -201,9 +222,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -236,6 +274,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -414,17 +469,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -432,7 +487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -440,7 +495,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -448,7 +503,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -456,7 +511,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -464,7 +519,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -472,7 +527,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -480,7 +535,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -488,13 +543,99 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="9.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Code v1.0 updated for gold rate test case
</commit_message>
<xml_diff>
--- a/Output/TestResult.xlsx
+++ b/Output/TestResult.xlsx
@@ -1,109 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ibmadmin\PycharmProjects\MoneyControl\Output\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="80" windowWidth="20120" windowHeight="8000" activeTab="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="80" windowWidth="20120" windowHeight="8000" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Currency" sheetId="1" r:id="rId1"/>
-    <sheet name="Gold Price" sheetId="2" r:id="rId2"/>
+    <sheet name="Currency" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Gold Price" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t>Currency Name</t>
-  </si>
-  <si>
-    <t>INR Converted</t>
-  </si>
-  <si>
-    <t>1 US $</t>
-  </si>
-  <si>
-    <t>73.0525</t>
-  </si>
-  <si>
-    <t>1 Euro €</t>
-  </si>
-  <si>
-    <t>88.8933</t>
-  </si>
-  <si>
-    <t>1 UK £</t>
-  </si>
-  <si>
-    <t>103.0069</t>
-  </si>
-  <si>
-    <t>1 Aus $</t>
-  </si>
-  <si>
-    <t>56.5353</t>
-  </si>
-  <si>
-    <t>1 Japanese ¥</t>
-  </si>
-  <si>
-    <t>0.6671</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 Singapore </t>
-  </si>
-  <si>
-    <t>55.1298</t>
-  </si>
-  <si>
-    <t>1 Renminbi</t>
-  </si>
-  <si>
-    <t>11.4302</t>
-  </si>
-  <si>
-    <t>1 Taiwan $</t>
-  </si>
-  <si>
-    <t>2.6397</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Change</t>
-  </si>
-  <si>
-    <t>%Change</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -121,28 +46,93 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -466,89 +456,129 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col width="14.7265625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="14" bestFit="1" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Currency Name</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>INR Converted</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>1 US $</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>73.0525</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>1 Euro €</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>88.8933</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>1 UK £</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>103.0069</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>1 Aus $</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>56.5353</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>1 Japanese ¥</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>0.6671</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 Singapore </t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>55.1298</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>1 Renminbi</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>11.4302</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>1 Taiwan $</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>2.6397</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -557,85 +587,132 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="9.08984375" customWidth="1"/>
+    <col width="11.08984375" customWidth="1" min="1" max="1"/>
+    <col width="11.1796875" customWidth="1" style="3" min="2" max="2"/>
+    <col width="12.36328125" customWidth="1" style="3" min="3" max="3"/>
+    <col width="10" customWidth="1" style="3" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Gold Price</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Price Change</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>%Change</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>05AUG2021</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>48880.00</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>-318.00</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="inlineStr">
+        <is>
+          <t>-0.65%</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>05OCT2021</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>49239.00</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>-247.00</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t>-0.50%</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n"/>
+      <c r="B4" s="1" t="n"/>
+      <c r="C4" s="1" t="n"/>
+      <c r="D4" s="1" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n"/>
+      <c r="B5" s="1" t="n"/>
+      <c r="C5" s="1" t="n"/>
+      <c r="D5" s="1" t="n"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n"/>
+      <c r="B6" s="1" t="n"/>
+      <c r="C6" s="1" t="n"/>
+      <c r="D6" s="1" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n"/>
+      <c r="B7" s="1" t="n"/>
+      <c r="C7" s="1" t="n"/>
+      <c r="D7" s="1" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n"/>
+      <c r="B8" s="1" t="n"/>
+      <c r="C8" s="1" t="n"/>
+      <c r="D8" s="1" t="n"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n"/>
+      <c r="B9" s="1" t="n"/>
+      <c r="C9" s="1" t="n"/>
+      <c r="D9" s="1" t="n"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n"/>
+      <c r="B10" s="1" t="n"/>
+      <c r="C10" s="1" t="n"/>
+      <c r="D10" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Code v1.1 updated after running all the tests. Minor modifications made.
</commit_message>
<xml_diff>
--- a/Output/TestResult.xlsx
+++ b/Output/TestResult.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="80" windowWidth="20120" windowHeight="8000" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="80" windowWidth="20120" windowHeight="8000" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Currency" sheetId="1" state="visible" r:id="rId1"/>
@@ -463,8 +463,8 @@
   </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="A2:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -493,7 +493,7 @@
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>73.0525</t>
+          <t>73.0675</t>
         </is>
       </c>
     </row>
@@ -505,7 +505,7 @@
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>88.8933</t>
+          <t>88.4809</t>
         </is>
       </c>
     </row>
@@ -517,7 +517,7 @@
       </c>
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>103.0069</t>
+          <t>103.0862</t>
         </is>
       </c>
     </row>
@@ -529,7 +529,7 @@
       </c>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>56.5353</t>
+          <t>56.3058</t>
         </is>
       </c>
     </row>
@@ -541,7 +541,7 @@
       </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>0.6671</t>
+          <t>0.6664</t>
         </is>
       </c>
     </row>
@@ -553,7 +553,7 @@
       </c>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>55.1298</t>
+          <t>55.1203</t>
         </is>
       </c>
     </row>
@@ -565,7 +565,7 @@
       </c>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>11.4302</t>
+          <t>11.4227</t>
         </is>
       </c>
     </row>
@@ -577,7 +577,7 @@
       </c>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>2.6397</t>
+          <t>2.6434</t>
         </is>
       </c>
     </row>
@@ -594,8 +594,8 @@
   </sheetPr>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
Code v1.0 updated for gratuity calculator test
</commit_message>
<xml_diff>
--- a/Output/TestResult.xlsx
+++ b/Output/TestResult.xlsx
@@ -636,17 +636,17 @@
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>48880.00</t>
+          <t>48501.00</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>-318.00</t>
+          <t>-402.00</t>
         </is>
       </c>
       <c r="D2" s="4" t="inlineStr">
         <is>
-          <t>-0.65%</t>
+          <t>-0.82%</t>
         </is>
       </c>
     </row>
@@ -658,17 +658,17 @@
       </c>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>49239.00</t>
+          <t>48815.00</t>
         </is>
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>-247.00</t>
+          <t>-410.00</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>-0.50%</t>
+          <t>-0.83%</t>
         </is>
       </c>
     </row>

</xml_diff>